<commit_message>
Korrektur des Entwurfes von UC-Intern
Umbenennen von Finalize in BuildGraph in der Klasse UseCase.
</commit_message>
<xml_diff>
--- a/02_Entwurf/UC-Intern/Schnittstelle_Beschreibungen_UC-Intern.xlsx
+++ b/02_Entwurf/UC-Intern/Schnittstelle_Beschreibungen_UC-Intern.xlsx
@@ -90,9 +90,6 @@
     <t>AddBoundedAlternativeFlow(id : int, steps : list&lt;string&gt;, postcondition : string, referenceSteps: List&lt;ReferenceStep&gt;) : void</t>
   </si>
   <si>
-    <t>Finalize() : void</t>
-  </si>
-  <si>
     <t>get_Nodes() : List&lt;Node&gt;</t>
   </si>
   <si>
@@ -157,22 +154,10 @@
     <t>get_StepDescription() : string</t>
   </si>
   <si>
-    <t>Finalizes the description of the use-case and allows for building the internal graph-representation. Before calling Finalize only the setters and methods starting with "Set" and "Add" are allowed to be called.
-After calling after using these methods to describe the use-case finalize is called and the given description is used to build a graph representation. After calling Finalize only the getters are allowed to be called.</t>
-  </si>
-  <si>
     <t>A flow identifier identifies one flow with a type and a number. As there is only one basic flow the number should not be accounted for the basic flow type.</t>
   </si>
   <si>
     <t>A reference step descibes one specific step across all flows and therefor has a flow identifier and a step number.</t>
-  </si>
-  <si>
-    <t>This class is used to create and retrieve the representation of the use-case as a graph. It also provides all the information contained in a use-case.
-The usage of the class involves two steps:
-The first step is to build the graph. For that the setter methods and the methods starting with "Set" and "Add" are used to insert the description of a graph. For that all "Set" methods must be used and all setters and "Add" methods can be used to describe a use-case.
-The setters (in this case setters are all methods starting with "set_" are not mandatory because they are simple string setters and therefor return null if no value was set.
-After inserting the whole description the method Finalize is called. After that no usage of setters, "Set" and "Add" methods is allowed anymore.
-The second step involves retrieval of the data. For that various getters are provided with most being simple string getters. The remaining getters are used to retrive the graph in a representation with a node list and two edge matrices.</t>
   </si>
   <si>
     <t>A condition describes the condition which must be matched for a edge in the graph to be valid. For most edges there is no condition meaning they are always valid (if the exists).
@@ -221,6 +206,21 @@
   </si>
   <si>
     <t>UseCase()</t>
+  </si>
+  <si>
+    <t>BuildGraph() : void</t>
+  </si>
+  <si>
+    <t>Signales the end of the description of the use-case and builds the internal graph-representation. Before calling BuildGraph only the setters and methods starting with "Set" and "Add" are allowed to be called.
+After using these methods to describe the use-case, BuildGraph is called and the given description is used to build a graph representation. After calling BuildGraph only the getters are allowed to be called.</t>
+  </si>
+  <si>
+    <t>This class is used to create and retrieve the representation of the use-case as a graph. It also provides all the information contained in a use-case.
+The usage of the class involves two steps:
+The first step is to build the graph. For that the setter methods and the methods starting with "Set" and "Add" are used to insert the description of a graph. For that all "Set" methods must be used and all setters and "Add" methods can be used to describe a use-case.
+The setters (in this case setters are all methods starting with "set_" are not mandatory because they are simple string setters and therefor return null if no value was set.
+After inserting the whole description the method BuildGraph is called. After that no usage of setters, "Set" and "Add" methods is allowed anymore.
+The second step involves retrieval of the data. For that various getters are provided with most being simple string getters. The remaining getters are used to retrive the graph in a representation with a node list and two edge matrices.</t>
   </si>
 </sst>
 </file>
@@ -562,9 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -579,12 +577,12 @@
     <row r="2" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -706,7 +704,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,7 +715,7 @@
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -728,7 +726,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,51 +737,51 @@
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +790,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B50" s="4"/>
     </row>
@@ -802,7 +800,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B52" s="4"/>
     </row>
@@ -812,7 +810,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B54" s="4"/>
     </row>
@@ -822,7 +820,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4"/>
     </row>
@@ -841,12 +839,12 @@
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,27 +852,27 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -885,22 +883,22 @@
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -911,17 +909,17 @@
     <row r="82" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -932,49 +930,49 @@
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>